<commit_message>
completed initial work on SW using FreqMeasure library. Required rewiring of board to pin PC7, will update in future SCH revision
</commit_message>
<xml_diff>
--- a/test-debug/meter-cal.xlsx
+++ b/test-debug/meter-cal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\NRG-Anemometer-Display\test-debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD845D4-4E0F-4839-AA33-68238FED5DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C4976A-32FB-40B7-B52C-B66B4D91DA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{A5091054-E6C2-47B0-9955-2837F76FFCC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Raw Freq</t>
+    <t>Freq</t>
   </si>
   <si>
-    <t>Cal 1</t>
+    <t>Meas</t>
   </si>
   <si>
-    <t>Cal 2</t>
+    <t>Ideal</t>
   </si>
   <si>
-    <t xml:space="preserve">Cal 3 </t>
+    <t>Cal Slope</t>
+  </si>
+  <si>
+    <t>Cal Offset</t>
+  </si>
+  <si>
+    <t>m/s to mph</t>
   </si>
 </sst>
 </file>
@@ -72,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -150,7 +157,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cal 1</c:v>
+                  <c:v>Meas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -169,186 +176,216 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$29</c:f>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>48</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$29</c:f>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>1.8580000000000001</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3759999999999999</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8940000000000001</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4119999999999999</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.93</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4480000000000004</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.965999999999999</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.484</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.002000000000001</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.52</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.038</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.556000000000001</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.074000000000002</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.591999999999999</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.11</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.628</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26.146000000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>27.664000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>29.181999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30.7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32.218000000000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>33.736000000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>35.254000000000005</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>36.772000000000006</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>38.290000000000006</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>39.808000000000007</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>41.326000000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>42.844000000000001</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -356,7 +393,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-14C9-4E01-89CD-CC3D7A68CDBA}"/>
+              <c16:uniqueId val="{00000001-A6CA-4776-B5A9-DCB262AB894B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -369,7 +406,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cal 2</c:v>
+                  <c:v>Ideal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -388,186 +425,318 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$29</c:f>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>48</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>50</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$29</c:f>
+              <c:f>Sheet1!$C$2:$C$51</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1.8900000000000001</c:v>
+                  <c:v>2.5255052600000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.41</c:v>
+                  <c:v>5.9211801800000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9300000000000006</c:v>
+                  <c:v>9.3168551000000015</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.45</c:v>
+                  <c:v>12.712530020000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.97</c:v>
+                  <c:v>16.108204940000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.49</c:v>
+                  <c:v>19.503879860000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.01</c:v>
+                  <c:v>22.899554780000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.53</c:v>
+                  <c:v>26.2952297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.049999999999999</c:v>
+                  <c:v>29.690904620000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.569999999999999</c:v>
+                  <c:v>33.086579540000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.09</c:v>
+                  <c:v>36.482254460000007</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.610000000000003</c:v>
+                  <c:v>39.877929380000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.130000000000003</c:v>
+                  <c:v>43.273604300000009</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.650000000000002</c:v>
+                  <c:v>46.66927922</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.17</c:v>
+                  <c:v>50.064954140000005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.69</c:v>
+                  <c:v>53.460629060000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26.21</c:v>
+                  <c:v>56.856303980000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.73</c:v>
+                  <c:v>60.251978900000012</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.25</c:v>
+                  <c:v>63.647653820000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.77</c:v>
+                  <c:v>67.043328740000007</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.29</c:v>
+                  <c:v>70.439003660000012</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>33.809999999999995</c:v>
+                  <c:v>73.834678580000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35.33</c:v>
+                  <c:v>77.230353500000007</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.85</c:v>
+                  <c:v>80.626028419999997</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>38.369999999999997</c:v>
+                  <c:v>84.021703340000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39.89</c:v>
+                  <c:v>87.417378260000007</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41.41</c:v>
+                  <c:v>90.813053180000011</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42.93</c:v>
+                  <c:v>94.208728100000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>97.604403019999992</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>101.00007794</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>104.39575286</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>107.79142778000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>111.1871027</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>114.58277762</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>117.97845254000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>121.37412746000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>124.76980238000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>128.16547729999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>131.56115222</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>134.95682714</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>138.35250206000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>141.74817698000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>145.14385190000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>148.53952682000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>151.93520174000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>155.33087666000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>158.72655158000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>162.12222650000004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>165.51790142000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>168.91357634000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,226 +744,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-14C9-4E01-89CD-CC3D7A68CDBA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cal 3 </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>1.8980000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.4159999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.9340000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.452</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.97</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.4880000000000013</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.524000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.042000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.56</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17.077999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18.596</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20.114000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21.631999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23.15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>24.667999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26.186</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>27.704000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>29.221999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30.74</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32.258000000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>33.776000000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>35.294000000000004</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>36.812000000000005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>38.330000000000005</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>39.848000000000006</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>41.366</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>42.884</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-14C9-4E01-89CD-CC3D7A68CDBA}"/>
+              <c16:uniqueId val="{00000002-A6CA-4776-B5A9-DCB262AB894B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -807,11 +757,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="39338031"/>
-        <c:axId val="156066863"/>
+        <c:axId val="18659519"/>
+        <c:axId val="18660351"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39338031"/>
+        <c:axId val="18659519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +804,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156066863"/>
+        <c:crossAx val="18660351"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -862,7 +812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156066863"/>
+        <c:axId val="18660351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39338031"/>
+        <c:crossAx val="18659519"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1561,22 +1511,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28FF3DE0-C0C0-4F37-86B3-B9A3327F83DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178E0406-693F-4D1B-9F0F-ED1D4661F676}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,7 +1564,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -1626,7 +1576,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -1673,6 +1623,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1708,6 +1675,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1859,16 +1843,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F1287E-5DCB-4B94-B8F7-375370A4D157}">
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1878,485 +1865,647 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <f>(A2*0.759) + 0.34</f>
-        <v>1.8580000000000001</v>
-      </c>
-      <c r="C2">
-        <f>(A2*0.76) + 0.37</f>
-        <v>1.8900000000000001</v>
-      </c>
-      <c r="D2">
-        <f>(A2*0.759) + 0.38</f>
-        <v>1.8980000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="1">
+        <f>((A2*$G$32)+$G$33)*$G$34</f>
+        <v>2.5255052600000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <f>((A3*$G$32)+$G$33)*$G$34</f>
+        <v>5.9211801800000012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <f>((A4*$G$32)+$G$33)*$G$34</f>
+        <v>9.3168551000000015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <f>((A5*$G$32)+$G$33)*$G$34</f>
+        <v>12.712530020000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <f>((A6*$G$32)+$G$33)*$G$34</f>
+        <v>16.108204940000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <f>((A7*$G$32)+$G$33)*$G$34</f>
+        <v>19.503879860000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <f>((A8*$G$32)+$G$33)*$G$34</f>
+        <v>22.899554780000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1">
+        <f>((A9*$G$32)+$G$33)*$G$34</f>
+        <v>26.2952297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <f>((A10*$G$32)+$G$33)*$G$34</f>
+        <v>29.690904620000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1">
+        <f>((A11*$G$32)+$G$33)*$G$34</f>
+        <v>33.086579540000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1">
+        <f>((A12*$G$32)+$G$33)*$G$34</f>
+        <v>36.482254460000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1">
+        <f>((A13*$G$32)+$G$33)*$G$34</f>
+        <v>39.877929380000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <f>((A14*$G$32)+$G$33)*$G$34</f>
+        <v>43.273604300000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1">
+        <f>((A15*$G$32)+$G$33)*$G$34</f>
+        <v>46.66927922</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1">
+        <f>((A16*$G$32)+$G$33)*$G$34</f>
+        <v>50.064954140000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1">
+        <f>((A17*$G$32)+$G$33)*$G$34</f>
+        <v>53.460629060000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1">
+        <f>((A18*$G$32)+$G$33)*$G$34</f>
+        <v>56.856303980000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1">
+        <f>((A19*$G$32)+$G$33)*$G$34</f>
+        <v>60.251978900000012</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1">
+        <f>((A20*$G$32)+$G$33)*$G$34</f>
+        <v>63.647653820000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1">
+        <f>((A21*$G$32)+$G$33)*$G$34</f>
+        <v>67.043328740000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1">
+        <f t="shared" ref="C22:C81" si="0">((A22*$G$32)+$G$33)*$G$34</f>
+        <v>70.439003660000012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>73.834678580000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>77.230353500000007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>80.626028419999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>84.021703340000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>87.417378260000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>53</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>90.813053180000011</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>94.208728100000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>57</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>97.604403019999992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>101.00007794</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>104.39575286</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>63</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>107.79142778000001</v>
+      </c>
+      <c r="F33" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B29" si="0">(A3*0.759) + 0.34</f>
-        <v>3.3759999999999999</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C29" si="1">(A3*0.76) + 0.37</f>
-        <v>3.41</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D29" si="2">(A3*0.759) + 0.38</f>
-        <v>3.4159999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>4.8940000000000001</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>4.9300000000000006</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="2"/>
-        <v>4.9340000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>6.4119999999999999</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>6.45</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="2"/>
-        <v>6.452</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>7.93</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>7.97</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="2"/>
-        <v>7.97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>9.4480000000000004</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>9.49</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="2"/>
-        <v>9.4880000000000013</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>10.965999999999999</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>11.01</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>11.006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>12.484</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>12.53</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>12.524000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>14.002000000000001</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>14.049999999999999</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>14.042000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>15.52</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>15.569999999999999</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>15.56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>17.038</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>17.09</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>17.077999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>18.556000000000001</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>18.610000000000003</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>18.596</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>26</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>20.074000000000002</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>20.130000000000003</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>20.114000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>21.591999999999999</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>21.650000000000002</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>21.631999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>30</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>23.11</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>23.17</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>23.15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>32</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>24.628</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>24.69</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>24.667999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>34</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>26.146000000000001</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>26.21</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>26.186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>36</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>27.664000000000001</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>27.73</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>27.704000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>38</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>29.181999999999999</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>29.25</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>29.221999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>40</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>30.7</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>30.77</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>30.74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>42</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>32.218000000000004</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>32.29</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>32.258000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>44</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>33.736000000000004</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
-        <v>33.809999999999995</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>33.776000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>46</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>35.254000000000005</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
-        <v>35.33</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>35.294000000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>48</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>36.772000000000006</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="1"/>
-        <v>36.85</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>36.812000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>50</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>38.290000000000006</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="1"/>
-        <v>38.369999999999997</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="2"/>
-        <v>38.330000000000005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>52</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>39.808000000000007</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="1"/>
-        <v>39.89</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="2"/>
-        <v>39.848000000000006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>54</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>41.326000000000001</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>41.41</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>41.366</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>56</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>42.844000000000001</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>42.93</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="2"/>
-        <v>42.884</v>
-      </c>
+      <c r="G33">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>111.1871027</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>2.2369400000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>67</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>114.58277762</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>117.97845254000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>71</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>121.37412746000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>73</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>124.76980238000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>75</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>128.16547729999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>77</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>131.56115222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1">
+        <f t="shared" si="0"/>
+        <v>134.95682714</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1">
+        <f t="shared" si="0"/>
+        <v>138.35250206000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>83</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>141.74817698000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1">
+        <f t="shared" si="0"/>
+        <v>145.14385190000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>87</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1">
+        <f t="shared" si="0"/>
+        <v>148.53952682000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>89</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1">
+        <f t="shared" si="0"/>
+        <v>151.93520174000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>91</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1">
+        <f t="shared" si="0"/>
+        <v>155.33087666000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>93</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>158.72655158000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>162.12222650000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>97</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1">
+        <f t="shared" si="0"/>
+        <v>165.51790142000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>99</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1">
+        <f t="shared" si="0"/>
+        <v>168.91357634000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>